<commit_message>
updated violin plot style to one per page
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niroren/ownCloud/scratch/marks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1DF7ECE9-D848-4A47-882F-7BE7A1A0A8FA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD80DA2-BA72-2F40-A846-FF6F42B4C4B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26640" yWindow="3680" windowWidth="25440" windowHeight="15000" xr2:uid="{10E1CCD1-3864-4749-BDFD-AA40C54CF694}"/>
+    <workbookView xWindow="14180" yWindow="1420" windowWidth="14300" windowHeight="15000" xr2:uid="{10E1CCD1-3864-4749-BDFD-AA40C54CF694}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,26 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
   <si>
     <t>filename</t>
   </si>
   <si>
-    <t>CS1520 Marksheet 2017-2018.xlsx</t>
-  </si>
-  <si>
-    <t>CS1522 Marksheet 2017-2018.xlsx</t>
-  </si>
-  <si>
-    <t>CS1524 Marksheet 2017-2018.xlsx</t>
-  </si>
-  <si>
-    <t>CS1525 Marksheet 2017-2018.xlsx</t>
-  </si>
-  <si>
-    <t>CS1527 Marksheet 2017-2018.xlsx</t>
-  </si>
-  <si>
     <t>Number of students</t>
   </si>
   <si>
@@ -57,9 +42,6 @@
     <t>CS1520</t>
   </si>
   <si>
-    <t>CS1522</t>
-  </si>
-  <si>
     <t>CS1524</t>
   </si>
   <si>
@@ -72,13 +54,226 @@
     <t>Marks column</t>
   </si>
   <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>W</t>
+    <t>CS1520 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS1524 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS1525 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS1527 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS2506 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS2510 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS2512 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS2521 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS3518 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS3524 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS3528 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS4525 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS4527 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS4594 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS551M Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS2510</t>
+  </si>
+  <si>
+    <t>CS2512</t>
+  </si>
+  <si>
+    <t>CS2521</t>
+  </si>
+  <si>
+    <t>CS3518</t>
+  </si>
+  <si>
+    <t>CS3524</t>
+  </si>
+  <si>
+    <t>CS3528</t>
+  </si>
+  <si>
+    <t>CS4525</t>
+  </si>
+  <si>
+    <t>CS4527</t>
+  </si>
+  <si>
+    <t>CS4594</t>
+  </si>
+  <si>
+    <t>CS551M</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>CS2506</t>
+  </si>
+  <si>
+    <t>CS1022 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS1024 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS1025 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS2012 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS2013 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS2014 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS2015 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS3025 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS3026 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS3027 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS3028 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS3525 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS4025 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS4028 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS4040 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS4046 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS4047 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS5059 Marksheet 2018-2019.xlsx</t>
+  </si>
+  <si>
+    <t>CS1022</t>
+  </si>
+  <si>
+    <t>CS1024</t>
+  </si>
+  <si>
+    <t>CS1025</t>
+  </si>
+  <si>
+    <t>CS2012</t>
+  </si>
+  <si>
+    <t>CS2013</t>
+  </si>
+  <si>
+    <t>CS2014</t>
+  </si>
+  <si>
+    <t>CS2015</t>
+  </si>
+  <si>
+    <t>CS3025</t>
+  </si>
+  <si>
+    <t>CS3026</t>
+  </si>
+  <si>
+    <t>CS3027</t>
+  </si>
+  <si>
+    <t>CS3028</t>
+  </si>
+  <si>
+    <t>CS3525</t>
+  </si>
+  <si>
+    <t>CS4025</t>
+  </si>
+  <si>
+    <t>CS4028</t>
+  </si>
+  <si>
+    <t>CS4040</t>
+  </si>
+  <si>
+    <t>CS4046</t>
+  </si>
+  <si>
+    <t>CS4047</t>
+  </si>
+  <si>
+    <t>CS5059</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -430,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C49477E-8616-4C4A-82A5-60FF55F5DBC1}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,101 +643,577 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>13</v>
       </c>
       <c r="C2">
-        <v>62</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>13</v>
       </c>
       <c r="C3">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
-      </c>
-      <c r="B5">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>14</v>
       </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29">
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>